<commit_message>
CRUD and Import Employee as User
</commit_message>
<xml_diff>
--- a/public/DataEmployee/custom_employee_template (3).xlsx
+++ b/public/DataEmployee/custom_employee_template (3).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acha\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5F3EEA-2990-47C5-92A0-007B8DDBCA2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD92BC21-5656-4B80-8F6E-BEDCDB8FC2F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>No</t>
   </si>
@@ -48,47 +48,32 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
     <t>Pangkat</t>
   </si>
   <si>
-    <t>kepala</t>
-  </si>
-  <si>
-    <t>Produksi</t>
-  </si>
-  <si>
-    <t>zakia</t>
-  </si>
-  <si>
-    <t>syahfitri</t>
-  </si>
-  <si>
-    <t>zakia@bps.go.id</t>
-  </si>
-  <si>
-    <t>sayang</t>
-  </si>
-  <si>
-    <t>sayang@bps.go.id</t>
-  </si>
-  <si>
-    <t>syahfitri@bps.go.id</t>
-  </si>
-  <si>
-    <t>saynng</t>
+    <t>Neraca</t>
+  </si>
+  <si>
+    <t>Aku</t>
+  </si>
+  <si>
+    <t>Kamu</t>
+  </si>
+  <si>
+    <t>aku@bps.go.id</t>
+  </si>
+  <si>
+    <t>kam@bps.go.id</t>
+  </si>
+  <si>
+    <t>anggota</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -99,11 +84,6 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -127,10 +107,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -436,131 +415,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="8.7265625" style="1"/>
-    <col min="2" max="2" width="15.7265625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="8.7265625" style="1"/>
-    <col min="5" max="5" width="18.08984375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
+      <c r="D2">
+        <v>123</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1">
-        <v>123</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="1">
-        <v>12345</v>
-      </c>
-      <c r="H2" s="1" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>789</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1">
-        <v>123</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="1">
-        <v>12345</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="F3" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="1">
-        <v>123</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="1">
-        <v>12345</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{CF6903AC-753F-4FD9-88E7-4D77631B4AA7}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{6390BA7A-7D04-4714-9151-DCE3857832AA}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{C912B4B2-BD43-40D5-BF64-EA7F4CEFC93B}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{01709901-2685-45E3-9DD7-41C2168CFD7E}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{058F1EBE-017A-44FF-8E62-1121540FE30F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>